<commit_message>
update printing function and minor bugs fixes
</commit_message>
<xml_diff>
--- a/data/col_test_data/toy_data_17May2021.xlsx
+++ b/data/col_test_data/toy_data_17May2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiwenzhang/Documents/GitHub/public_data_food_analysis_3/data/col_test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279FE007-85E8-2C4D-8DDC-D3F087237722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA91CD58-483D-3B4A-A4E5-309E3BAA6C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>mCC_ID</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>yrt1999</t>
+  </si>
+  <si>
+    <t>yrt2000</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
   <dimension ref="A1:ALO984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3908,14 +3911,30 @@
       <c r="ALO3" s="9"/>
     </row>
     <row r="4" spans="1:1003" ht="15.75" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="A4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10">
+        <v>44328</v>
+      </c>
+      <c r="F4" s="10">
+        <v>44330</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>

</xml_diff>